<commit_message>
added link and updated results
</commit_message>
<xml_diff>
--- a/results_overview.xlsx
+++ b/results_overview.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="0" windowWidth="27705" windowHeight="14220"/>
+    <workbookView xWindow="2190" yWindow="0" windowWidth="27705" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -145,13 +145,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -161,11 +166,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -498,27 +498,27 @@
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="3" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="3" t="s">
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
     </row>
     <row r="5" spans="1:17">
       <c r="C5" t="s">
@@ -599,7 +599,7 @@
         <v>30509</v>
       </c>
       <c r="K6" s="2">
-        <v>16.73</v>
+        <v>11.41</v>
       </c>
       <c r="L6" s="2">
         <v>9</v>
@@ -614,7 +614,7 @@
         <v>129631</v>
       </c>
       <c r="P6" s="2">
-        <v>125.75</v>
+        <v>51.68</v>
       </c>
       <c r="Q6" s="2">
         <v>12</v>
@@ -642,20 +642,20 @@
       <c r="G7">
         <v>6</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="6" t="s">
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="8"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="11"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8">
@@ -732,20 +732,20 @@
       <c r="G9">
         <v>50</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="6" t="s">
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="8"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="11"/>
     </row>
     <row r="10" spans="1:17">
       <c r="A10">
@@ -822,20 +822,20 @@
       <c r="G11">
         <v>6</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="6" t="s">
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="8"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="11"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12">
@@ -1012,7 +1012,7 @@
       <c r="E15">
         <v>50</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="3">
         <v>1</v>
       </c>
       <c r="G15">
@@ -1033,33 +1033,33 @@
       <c r="L15" s="2">
         <v>9</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="4">
         <v>228</v>
       </c>
-      <c r="N15" s="11">
+      <c r="N15" s="5">
         <v>230</v>
       </c>
-      <c r="O15" s="11">
+      <c r="O15" s="5">
         <v>2072</v>
       </c>
-      <c r="P15" s="11">
+      <c r="P15" s="5">
         <v>323.14</v>
       </c>
-      <c r="Q15" s="11">
+      <c r="Q15" s="5">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="M11:Q11"/>
+    <mergeCell ref="M9:Q9"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="H4:L4"/>
     <mergeCell ref="M4:Q4"/>
     <mergeCell ref="H7:L7"/>
     <mergeCell ref="H9:L9"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="M11:Q11"/>
-    <mergeCell ref="M9:Q9"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:G15">
     <cfRule type="colorScale" priority="6">
@@ -1085,7 +1085,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 L8 L10 L12:L15">
+  <conditionalFormatting sqref="L8 L6 L10 L12:L15">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1109,7 +1109,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P6 P8 P10 P12:P14 P15">
+  <conditionalFormatting sqref="P8 P6 P10 P12:P14 P15">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>